<commit_message>
Loading D20MEII WinPt Document Via Tkinter
When running the program, the code now opens the D20 WinPt Excel check sheet using tkinter. Much more user friendly.
</commit_message>
<xml_diff>
--- a/Example D20 XML/D20M++/FE D20 M++ QC Doc Rev 3.xlsx
+++ b/Example D20 XML/D20M++/FE D20 M++ QC Doc Rev 3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="345">
   <si>
     <t>D20 ME,  MEII and MX QC Document</t>
   </si>
@@ -168,6 +168,9 @@
     <t>RESTART DELAY</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>B023_DEV</t>
   </si>
   <si>
@@ -177,27 +180,42 @@
     <t>5 sec</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>INTEGRITY POLL INTERVAL</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>OFFLINE AFTER FAIL</t>
   </si>
   <si>
     <t>OFFLINE AFTER CHAN. FAIL</t>
   </si>
   <si>
+    <t>Off-line after chan fail</t>
+  </si>
+  <si>
     <t>FAILURES FOR BAD CHAN.</t>
   </si>
   <si>
     <t>3 (minimum)</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>TIMESYNCING</t>
   </si>
   <si>
     <t>DISABLE</t>
   </si>
   <si>
+    <t>Disable</t>
+  </si>
+  <si>
     <t>HARRIS DCA</t>
   </si>
   <si>
@@ -315,9 +333,6 @@
     <t>Standard UTC Offset</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>DST Offset</t>
   </si>
   <si>
@@ -357,9 +372,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>PLEASANT VALLEY SUBSTATION     SAB0605/03</t>
   </si>
   <si>
@@ -384,9 +396,6 @@
     <t>Port 3 - Spare</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Port 4 - DNP3.0 DPA SAM-900 HMI, 9600 baud</t>
   </si>
   <si>
@@ -465,9 +474,6 @@
     <t>501</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>1F5</t>
   </si>
   <si>
@@ -870,9 +876,6 @@
     <t>DCD, RTS, &amp; CTS</t>
   </si>
   <si>
-    <t>Disable</t>
-  </si>
-  <si>
     <t>DCD to RX enable time</t>
   </si>
   <si>
@@ -916,6 +919,9 @@
   </si>
   <si>
     <t>Confirm Required</t>
+  </si>
+  <si>
+    <t>Confirm Not Required</t>
   </si>
   <si>
     <t xml:space="preserve">After the Config is done, go back and make sure the WinPoints in the Points List were updated to reflect the new equipment or changes and match what is in the Config File. </t>
@@ -4688,7 +4694,7 @@
       <c r="I33" s="128" t="n"/>
       <c r="J33" s="128" t="n"/>
       <c r="L33" s="173" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
     </row>
     <row customFormat="1" r="34" s="147" spans="1:22">
@@ -4696,35 +4702,37 @@
         <v>29</v>
       </c>
       <c r="C34" s="91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" s="91" t="s">
         <v>31</v>
       </c>
       <c r="E34" s="91" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F34" s="91" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G34" s="91" t="n"/>
       <c r="H34" s="128" t="n"/>
       <c r="I34" s="128" t="n"/>
       <c r="J34" s="128" t="n"/>
-      <c r="L34" s="173" t="n"/>
+      <c r="L34" s="173" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row customFormat="1" r="35" s="147" spans="1:22">
       <c r="B35" s="91" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" s="91" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="91" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F35" s="91" t="n">
         <v>0</v>
@@ -4733,73 +4741,81 @@
       <c r="H35" s="128" t="n"/>
       <c r="I35" s="128" t="n"/>
       <c r="J35" s="128" t="n"/>
-      <c r="L35" s="173" t="n"/>
+      <c r="L35" s="173" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row customFormat="1" r="36" s="147" spans="1:22">
       <c r="B36" s="91" t="s">
         <v>29</v>
       </c>
       <c r="C36" s="91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" s="72" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="91" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F36" s="91" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G36" s="91" t="n"/>
       <c r="H36" s="128" t="n"/>
       <c r="I36" s="128" t="n"/>
       <c r="J36" s="128" t="n"/>
-      <c r="L36" s="173" t="n"/>
+      <c r="L36" s="173" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row customFormat="1" r="37" s="147" spans="1:22">
       <c r="B37" s="91" t="s">
         <v>29</v>
       </c>
       <c r="C37" s="91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D37" s="91" t="s">
         <v>31</v>
       </c>
       <c r="E37" s="91" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F37" s="91" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G37" s="91" t="n"/>
       <c r="H37" s="128" t="n"/>
       <c r="I37" s="128" t="n"/>
       <c r="J37" s="128" t="n"/>
-      <c r="L37" s="173" t="n"/>
+      <c r="L37" s="173" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row customFormat="1" r="38" s="147" spans="1:22">
       <c r="B38" s="91" t="s">
         <v>29</v>
       </c>
       <c r="C38" s="91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" s="91" t="s">
         <v>31</v>
       </c>
       <c r="E38" s="91" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F38" s="91" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G38" s="91" t="n"/>
       <c r="H38" s="128" t="n"/>
       <c r="I38" s="128" t="n"/>
       <c r="J38" s="128" t="n"/>
-      <c r="L38" s="173" t="n"/>
+      <c r="L38" s="173" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row customFormat="1" r="39" s="147" spans="1:22">
       <c r="B39" s="91" t="n"/>
@@ -4815,16 +4831,16 @@
     </row>
     <row customFormat="1" r="40" s="147" spans="1:22">
       <c r="B40" s="91" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C40" s="91" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D40" s="91" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E40" s="91" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F40" s="91" t="n">
         <v>5</v>
@@ -4834,7 +4850,7 @@
       <c r="I40" s="128" t="n"/>
       <c r="J40" s="128" t="n"/>
       <c r="L40" s="173" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row customFormat="1" r="41" s="147" spans="1:22">
@@ -4851,43 +4867,43 @@
     </row>
     <row customFormat="1" r="42" s="147" spans="1:22">
       <c r="B42" s="91" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C42" s="91" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D42" s="91" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E42" s="91" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F42" s="91" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G42" s="91" t="n"/>
       <c r="H42" s="128" t="n"/>
       <c r="I42" s="128" t="n"/>
       <c r="J42" s="128" t="n"/>
       <c r="L42" s="173" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row customFormat="1" r="43" s="147" spans="1:22">
       <c r="B43" s="91" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C43" s="91" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D43" s="91" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E43" s="91" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F43" s="91" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G43" s="91" t="n"/>
       <c r="H43" s="128" t="n"/>
@@ -4911,7 +4927,7 @@
       <c r="B45" s="28" t="n"/>
       <c r="C45" s="29" t="n"/>
       <c r="D45" s="149" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F45" s="16" t="n"/>
       <c r="G45" s="91" t="n"/>
@@ -4924,7 +4940,7 @@
       <c r="B46" s="30" t="n"/>
       <c r="C46" s="91" t="n"/>
       <c r="D46" s="157" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F46" s="66" t="n"/>
       <c r="G46" s="91" t="n"/>
@@ -4949,18 +4965,18 @@
     <row customFormat="1" r="48" s="147" spans="1:22">
       <c r="A48" s="110" t="n"/>
       <c r="B48" s="157" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C48" s="91" t="n"/>
       <c r="D48" s="13" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E48" s="10">
         <f>C65</f>
         <v/>
       </c>
       <c r="F48" s="148" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G48" s="91" t="n"/>
       <c r="H48" s="128" t="n"/>
@@ -4972,7 +4988,7 @@
       <c r="A49" s="110" t="n"/>
       <c r="C49" s="91" t="n"/>
       <c r="D49" s="14" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E49" s="10">
         <f>D65</f>
@@ -4988,7 +5004,7 @@
       <c r="A50" s="110" t="n"/>
       <c r="C50" s="91" t="n"/>
       <c r="D50" s="14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E50" s="10">
         <f>B65</f>
@@ -5004,7 +5020,7 @@
       <c r="A51" s="110" t="n"/>
       <c r="C51" s="91" t="n"/>
       <c r="D51" s="15" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E51" s="10">
         <f>F65</f>
@@ -5031,7 +5047,7 @@
     </row>
     <row customFormat="1" r="53" s="147" spans="1:22">
       <c r="B53" s="161" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G53" s="30" t="n"/>
       <c r="H53" s="128" t="n"/>
@@ -5053,19 +5069,19 @@
     </row>
     <row customFormat="1" r="55" s="147" spans="1:22">
       <c r="B55" s="17" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F55" s="108" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G55" s="30" t="n"/>
       <c r="H55" s="128" t="n"/>
@@ -5266,16 +5282,16 @@
     </row>
     <row customFormat="1" r="67" s="147" spans="1:22">
       <c r="B67" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C67" s="91" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D67" s="91" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E67" s="91" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F67" s="91" t="n">
         <v>500</v>
@@ -5285,45 +5301,45 @@
       <c r="I67" s="128" t="n"/>
       <c r="J67" s="128" t="n"/>
       <c r="L67" s="173" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="13.2" r="68" s="147" spans="1:22">
       <c r="B68" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C68" s="91" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D68" s="91" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E68" s="91" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F68" s="91" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G68" s="91" t="n"/>
       <c r="H68" s="128" t="n"/>
       <c r="I68" s="128" t="n"/>
       <c r="J68" s="128" t="n"/>
       <c r="L68" s="173" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row customFormat="1" r="69" s="147" spans="1:22">
       <c r="B69" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C69" s="91" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D69" s="91" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E69" s="91" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F69" s="91" t="n">
         <v>0</v>
@@ -5333,21 +5349,21 @@
       <c r="I69" s="128" t="n"/>
       <c r="J69" s="128" t="n"/>
       <c r="L69" s="173" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row customFormat="1" r="70" s="147" spans="1:22">
       <c r="B70" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C70" s="91" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D70" s="91" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E70" s="91" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F70" s="91" t="n">
         <v>0</v>
@@ -5357,21 +5373,21 @@
       <c r="I70" s="128" t="n"/>
       <c r="J70" s="128" t="n"/>
       <c r="L70" s="173" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row customFormat="1" r="71" s="147" spans="1:22">
       <c r="B71" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C71" s="91" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D71" s="91" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E71" s="91" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F71" s="91" t="n"/>
       <c r="G71" s="91" t="n"/>
@@ -5379,21 +5395,21 @@
       <c r="I71" s="128" t="n"/>
       <c r="J71" s="128" t="n"/>
       <c r="L71" s="173" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row customFormat="1" r="72" s="147" spans="1:22">
       <c r="B72" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C72" s="91" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D72" s="91" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E72" s="91" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F72" s="91" t="n"/>
       <c r="G72" s="91" t="n"/>
@@ -5403,16 +5419,16 @@
     </row>
     <row customFormat="1" r="73" s="147" spans="1:22">
       <c r="B73" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C73" s="91" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D73" s="91" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E73" s="91" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F73" s="91" t="n"/>
       <c r="G73" s="91" t="n"/>
@@ -5422,19 +5438,19 @@
     </row>
     <row customFormat="1" r="74" s="147" spans="1:22">
       <c r="B74" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C74" s="91" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D74" s="91" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E74" s="91" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F74" s="91" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G74" s="91" t="n"/>
       <c r="H74" s="128" t="n"/>
@@ -5444,13 +5460,13 @@
     </row>
     <row customFormat="1" r="75" s="147" spans="1:22">
       <c r="B75" s="91" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C75" s="91" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D75" s="91" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G75" s="91" t="n"/>
       <c r="L75" s="137" t="n"/>
@@ -5466,10 +5482,10 @@
     <row customFormat="1" r="77" s="147" spans="1:22">
       <c r="B77" s="91" t="n"/>
       <c r="C77" s="87" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D77" s="167" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F77" s="160" t="n"/>
       <c r="G77" s="91" t="n"/>
@@ -5478,13 +5494,13 @@
     <row customFormat="1" r="78" s="147" spans="1:22">
       <c r="B78" s="91" t="n"/>
       <c r="C78" s="132" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="D78" s="174" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F78" s="159" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G78" s="91" t="n"/>
       <c r="H78" s="128" t="n"/>
@@ -5495,10 +5511,10 @@
     <row customFormat="1" r="79" s="147" spans="1:22">
       <c r="B79" s="91" t="n"/>
       <c r="C79" s="133" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D79" s="169" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G79" s="91" t="n"/>
       <c r="I79" s="128" t="n"/>
@@ -5507,10 +5523,10 @@
     <row customFormat="1" r="80" s="147" spans="1:22">
       <c r="B80" s="91" t="n"/>
       <c r="C80" s="133" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D80" s="169" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G80" s="91" t="n"/>
       <c r="I80" s="128" t="n"/>
@@ -5519,10 +5535,10 @@
     <row customFormat="1" r="81" s="147" spans="1:22">
       <c r="B81" s="91" t="n"/>
       <c r="C81" s="133" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D81" s="169" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G81" s="91" t="n"/>
       <c r="I81" s="128" t="n"/>
@@ -5531,10 +5547,10 @@
     <row customFormat="1" r="82" s="147" spans="1:22">
       <c r="B82" s="91" t="n"/>
       <c r="C82" s="133" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="D82" s="169" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F82" s="160" t="n"/>
       <c r="G82" s="91" t="n"/>
@@ -5547,7 +5563,7 @@
         <v>43</v>
       </c>
       <c r="D83" s="169" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F83" s="160" t="n"/>
       <c r="G83" s="91" t="n"/>
@@ -5557,10 +5573,10 @@
     <row customFormat="1" r="84" s="147" spans="1:22">
       <c r="B84" s="91" t="n"/>
       <c r="C84" s="133" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D84" s="169" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F84" s="160" t="n"/>
       <c r="G84" s="91" t="n"/>
@@ -5570,10 +5586,10 @@
     <row customFormat="1" r="85" s="147" spans="1:22">
       <c r="B85" s="91" t="n"/>
       <c r="C85" s="133" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D85" s="169" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F85" s="160" t="n"/>
       <c r="G85" s="91" t="n"/>
@@ -5583,10 +5599,10 @@
     <row customFormat="1" r="86" s="147" spans="1:22">
       <c r="B86" s="91" t="n"/>
       <c r="C86" s="133" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D86" s="169" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F86" s="160" t="n"/>
       <c r="G86" s="91" t="n"/>
@@ -5811,16 +5827,16 @@
     </row>
     <row customFormat="1" r="110" s="147" spans="1:22">
       <c r="B110" s="91" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C110" s="91" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D110" s="91" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E110" s="72" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F110" s="72" t="n">
         <v>10</v>
@@ -5830,7 +5846,7 @@
       <c r="I110" s="128" t="n"/>
       <c r="J110" s="128" t="n"/>
       <c r="L110" s="173" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row customFormat="1" r="111" s="147" spans="1:22">
@@ -5849,13 +5865,13 @@
       <c r="B112" s="91" t="n"/>
       <c r="C112" s="91" t="n"/>
       <c r="D112" s="158" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E112" s="158" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F112" s="158" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G112" s="72" t="n"/>
       <c r="H112" s="128" t="n"/>
@@ -5864,99 +5880,99 @@
     </row>
     <row customFormat="1" r="113" s="147" spans="1:22">
       <c r="B113" s="91" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C113" s="91" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D113" s="158" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E113" s="158" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F113" s="63" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G113" s="72" t="n"/>
       <c r="H113" s="128" t="n"/>
       <c r="I113" s="128" t="n"/>
       <c r="J113" s="128" t="n"/>
       <c r="L113" s="90" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row customFormat="1" r="114" s="147" spans="1:22">
       <c r="B114" s="91" t="n"/>
       <c r="C114" s="91" t="n"/>
       <c r="D114" s="64" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E114" s="62" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="F114" s="43" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="G114" s="72" t="n"/>
       <c r="H114" s="128" t="n"/>
       <c r="I114" s="128" t="n"/>
       <c r="J114" s="128" t="n"/>
       <c r="L114" s="88" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row customFormat="1" r="115" s="147" spans="1:22">
       <c r="B115" s="91" t="n"/>
       <c r="C115" s="91" t="n"/>
       <c r="D115" s="64" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E115" s="62" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F115" s="43" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G115" s="72" t="n"/>
       <c r="H115" s="128" t="n"/>
       <c r="I115" s="128" t="n"/>
       <c r="J115" s="128" t="n"/>
       <c r="L115" s="88" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row customFormat="1" r="116" s="147" spans="1:22">
       <c r="B116" s="91" t="n"/>
       <c r="C116" s="91" t="n"/>
       <c r="D116" s="62" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E116" s="62" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F116" s="43" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G116" s="72" t="n"/>
       <c r="H116" s="128" t="n"/>
       <c r="I116" s="128" t="n"/>
       <c r="J116" s="128" t="n"/>
       <c r="L116" s="88" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row customFormat="1" r="117" s="147" spans="1:22">
       <c r="B117" s="91" t="n"/>
       <c r="C117" s="91" t="n"/>
       <c r="D117" s="62" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E117" s="62" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="F117" s="43" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G117" s="72" t="n"/>
       <c r="H117" s="128" t="n"/>
@@ -5964,20 +5980,20 @@
       <c r="J117" s="128" t="n"/>
       <c r="K117" s="65" t="n"/>
       <c r="L117" s="88" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="118" s="147" spans="1:22">
       <c r="B118" s="91" t="n"/>
       <c r="C118" s="91" t="n"/>
       <c r="D118" s="62" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="E118" s="62" t="s">
         <v>44</v>
       </c>
       <c r="F118" s="43" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G118" s="72" t="n"/>
       <c r="H118" s="128" t="n"/>
@@ -5985,7 +6001,7 @@
       <c r="J118" s="128" t="n"/>
       <c r="K118" s="65" t="n"/>
       <c r="L118" s="88" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:22">
@@ -6040,13 +6056,13 @@
       <c r="B122" s="91" t="n"/>
       <c r="C122" s="91" t="n"/>
       <c r="D122" s="158" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E122" s="158" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F122" s="158" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G122" s="72" t="n"/>
       <c r="H122" s="128" t="n"/>
@@ -6058,19 +6074,19 @@
     </row>
     <row r="123" spans="1:22">
       <c r="B123" s="91" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C123" s="91" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D123" s="158" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E123" s="158" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F123" s="72" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G123" s="72" t="n"/>
       <c r="H123" s="128" t="n"/>
@@ -6078,7 +6094,7 @@
       <c r="J123" s="128" t="n"/>
       <c r="K123" s="147" t="n"/>
       <c r="L123" s="90" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="M123" s="147" t="n"/>
     </row>
@@ -6086,13 +6102,13 @@
       <c r="B124" s="91" t="n"/>
       <c r="C124" s="91" t="n"/>
       <c r="D124" s="62" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E124" s="62" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="F124" s="43" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G124" s="72" t="n"/>
       <c r="H124" s="128" t="n"/>
@@ -6100,7 +6116,7 @@
       <c r="J124" s="128" t="n"/>
       <c r="K124" s="147" t="n"/>
       <c r="L124" s="88" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M124" s="147" t="n"/>
     </row>
@@ -6108,60 +6124,60 @@
       <c r="B125" s="91" t="n"/>
       <c r="C125" s="91" t="n"/>
       <c r="D125" s="62" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E125" s="62" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F125" s="43" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G125" s="72" t="n"/>
       <c r="H125" s="128" t="n"/>
       <c r="I125" s="128" t="n"/>
       <c r="J125" s="128" t="n"/>
       <c r="L125" s="88" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row customFormat="1" r="126" s="147" spans="1:22">
       <c r="B126" s="91" t="n"/>
       <c r="C126" s="91" t="n"/>
       <c r="D126" s="62" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="E126" s="62" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F126" s="43" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G126" s="72" t="n"/>
       <c r="H126" s="128" t="n"/>
       <c r="I126" s="128" t="n"/>
       <c r="J126" s="128" t="n"/>
       <c r="L126" s="88" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row customFormat="1" r="127" s="147" spans="1:22">
       <c r="B127" s="91" t="n"/>
       <c r="C127" s="91" t="n"/>
       <c r="D127" s="62" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E127" s="62" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="F127" s="43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G127" s="72" t="n"/>
       <c r="H127" s="128" t="n"/>
       <c r="I127" s="128" t="n"/>
       <c r="J127" s="128" t="n"/>
       <c r="L127" s="88" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="128" s="147" spans="1:22">
@@ -6174,14 +6190,14 @@
         <v>44</v>
       </c>
       <c r="F128" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G128" s="72" t="n"/>
       <c r="H128" s="128" t="n"/>
       <c r="I128" s="128" t="n"/>
       <c r="J128" s="128" t="n"/>
       <c r="L128" s="88" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="129" spans="1:22">
@@ -6302,13 +6318,13 @@
     </row>
     <row r="136" spans="1:22">
       <c r="B136" s="91" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C136" s="91" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D136" s="158" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G136" s="158" t="n"/>
       <c r="H136" s="128" t="n"/>
@@ -6334,19 +6350,19 @@
     </row>
     <row r="138" spans="1:22">
       <c r="B138" s="94" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C138" s="97" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D138" s="95" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E138" s="96" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F138" s="98" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G138" s="91" t="n"/>
       <c r="H138" s="128" t="n"/>
@@ -6354,7 +6370,7 @@
       <c r="J138" s="128" t="n"/>
       <c r="K138" s="147" t="n"/>
       <c r="L138" s="173" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="M138" s="147" t="n"/>
     </row>
@@ -6363,16 +6379,16 @@
         <v>0</v>
       </c>
       <c r="C139" s="102" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D139" s="102" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E139" s="102" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F139" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G139" s="91" t="n"/>
       <c r="H139" s="128" t="n"/>
@@ -6387,16 +6403,16 @@
         <v>1</v>
       </c>
       <c r="C140" s="103" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D140" s="103" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E140" s="103" t="s">
+        <v>177</v>
+      </c>
+      <c r="F140" s="92" t="s">
         <v>175</v>
-      </c>
-      <c r="F140" s="92" t="s">
-        <v>173</v>
       </c>
       <c r="G140" s="91" t="n"/>
       <c r="H140" s="128" t="n"/>
@@ -6414,13 +6430,13 @@
         <v>39</v>
       </c>
       <c r="D141" s="103" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E141" s="103" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F141" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G141" s="91" t="n"/>
       <c r="H141" s="128" t="n"/>
@@ -6438,13 +6454,13 @@
         <v>39</v>
       </c>
       <c r="D142" s="103" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E142" s="103" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F142" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G142" s="91" t="n"/>
       <c r="H142" s="128" t="n"/>
@@ -6459,16 +6475,16 @@
         <v>4</v>
       </c>
       <c r="C143" s="103" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D143" s="103" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E143" s="103" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F143" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G143" s="91" t="n"/>
       <c r="H143" s="128" t="n"/>
@@ -6483,16 +6499,16 @@
         <v>5</v>
       </c>
       <c r="C144" s="103" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D144" s="103" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E144" s="103" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F144" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G144" s="91" t="n"/>
       <c r="H144" s="128" t="n"/>
@@ -6510,13 +6526,13 @@
         <v>39</v>
       </c>
       <c r="D145" s="103" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E145" s="103" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F145" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G145" s="91" t="n"/>
       <c r="H145" s="128" t="n"/>
@@ -6534,13 +6550,13 @@
         <v>39</v>
       </c>
       <c r="D146" s="103" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E146" s="103" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F146" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G146" s="91" t="n"/>
       <c r="H146" s="128" t="n"/>
@@ -6558,13 +6574,13 @@
         <v>39</v>
       </c>
       <c r="D147" s="103" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E147" s="103" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F147" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G147" s="91" t="n"/>
       <c r="H147" s="128" t="n"/>
@@ -6582,13 +6598,13 @@
         <v>39</v>
       </c>
       <c r="D148" s="103" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E148" s="103" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F148" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G148" s="91" t="n"/>
       <c r="H148" s="128" t="n"/>
@@ -6606,13 +6622,13 @@
         <v>39</v>
       </c>
       <c r="D149" s="103" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E149" s="103" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F149" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G149" s="91" t="n"/>
       <c r="H149" s="128" t="n"/>
@@ -6630,13 +6646,13 @@
         <v>39</v>
       </c>
       <c r="D150" s="103" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E150" s="103" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F150" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G150" s="91" t="n"/>
       <c r="H150" s="128" t="n"/>
@@ -6654,13 +6670,13 @@
         <v>39</v>
       </c>
       <c r="D151" s="103" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E151" s="103" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F151" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G151" s="91" t="n"/>
       <c r="H151" s="128" t="n"/>
@@ -6678,13 +6694,13 @@
         <v>39</v>
       </c>
       <c r="D152" s="103" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E152" s="103" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F152" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G152" s="91" t="n"/>
       <c r="H152" s="128" t="n"/>
@@ -6702,13 +6718,13 @@
         <v>39</v>
       </c>
       <c r="D153" s="103" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E153" s="103" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F153" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G153" s="91" t="n"/>
       <c r="H153" s="128" t="n"/>
@@ -6726,13 +6742,13 @@
         <v>39</v>
       </c>
       <c r="D154" s="103" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E154" s="103" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F154" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G154" s="91" t="n"/>
       <c r="H154" s="128" t="n"/>
@@ -6750,13 +6766,13 @@
         <v>39</v>
       </c>
       <c r="D155" s="103" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E155" s="103" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F155" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G155" s="91" t="n"/>
       <c r="H155" s="128" t="n"/>
@@ -6774,13 +6790,13 @@
         <v>39</v>
       </c>
       <c r="D156" s="103" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E156" s="103" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F156" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G156" s="91" t="n"/>
       <c r="H156" s="128" t="n"/>
@@ -6798,13 +6814,13 @@
         <v>39</v>
       </c>
       <c r="D157" s="103" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E157" s="103" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F157" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G157" s="91" t="n"/>
       <c r="H157" s="128" t="n"/>
@@ -6822,13 +6838,13 @@
         <v>39</v>
       </c>
       <c r="D158" s="103" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E158" s="103" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F158" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G158" s="91" t="n"/>
       <c r="H158" s="128" t="n"/>
@@ -6846,13 +6862,13 @@
         <v>39</v>
       </c>
       <c r="D159" s="103" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E159" s="103" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F159" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G159" s="91" t="n"/>
       <c r="H159" s="128" t="n"/>
@@ -6870,13 +6886,13 @@
         <v>39</v>
       </c>
       <c r="D160" s="103" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E160" s="103" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F160" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G160" s="91" t="n"/>
       <c r="H160" s="128" t="n"/>
@@ -6894,13 +6910,13 @@
         <v>39</v>
       </c>
       <c r="D161" s="103" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E161" s="103" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F161" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G161" s="91" t="n"/>
       <c r="H161" s="128" t="n"/>
@@ -6918,13 +6934,13 @@
         <v>39</v>
       </c>
       <c r="D162" s="103" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E162" s="103" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F162" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G162" s="91" t="n"/>
       <c r="H162" s="128" t="n"/>
@@ -6942,13 +6958,13 @@
         <v>39</v>
       </c>
       <c r="D163" s="103" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E163" s="103" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F163" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G163" s="91" t="n"/>
       <c r="H163" s="128" t="n"/>
@@ -6966,13 +6982,13 @@
         <v>39</v>
       </c>
       <c r="D164" s="103" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E164" s="103" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F164" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G164" s="91" t="n"/>
       <c r="H164" s="128" t="n"/>
@@ -6990,13 +7006,13 @@
         <v>39</v>
       </c>
       <c r="D165" s="103" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E165" s="103" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F165" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G165" s="91" t="n"/>
       <c r="H165" s="128" t="n"/>
@@ -7014,13 +7030,13 @@
         <v>39</v>
       </c>
       <c r="D166" s="103" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E166" s="103" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F166" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G166" s="91" t="n"/>
       <c r="H166" s="128" t="n"/>
@@ -7038,13 +7054,13 @@
         <v>39</v>
       </c>
       <c r="D167" s="103" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E167" s="103" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F167" s="92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G167" s="91" t="n"/>
       <c r="H167" s="128" t="n"/>
@@ -7097,50 +7113,50 @@
     </row>
     <row r="171" spans="1:22">
       <c r="B171" s="91" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C171" s="91" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D171" s="91" t="s">
         <v>47</v>
       </c>
       <c r="E171" s="91" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F171" s="91" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G171" s="91" t="n"/>
       <c r="H171" s="128" t="n"/>
       <c r="I171" s="128" t="n"/>
       <c r="J171" s="128" t="n"/>
       <c r="L171" s="173" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="172" spans="1:22">
       <c r="B172" s="91" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C172" s="91" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D172" s="91" t="s">
         <v>47</v>
       </c>
       <c r="E172" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="F172" s="91" t="s">
         <v>233</v>
-      </c>
-      <c r="F172" s="91" t="s">
-        <v>231</v>
       </c>
       <c r="G172" s="91" t="n"/>
       <c r="H172" s="128" t="n"/>
       <c r="I172" s="128" t="n"/>
       <c r="J172" s="128" t="n"/>
       <c r="L172" s="173" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="173" spans="1:22">
@@ -7175,7 +7191,7 @@
       <c r="B175" s="42" t="n"/>
       <c r="C175" s="166" t="n"/>
       <c r="D175" s="166" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F175" s="166" t="n"/>
       <c r="G175" s="164" t="n"/>
@@ -7188,16 +7204,16 @@
     </row>
     <row customHeight="1" ht="13.5" r="176" s="140" spans="1:22" thickBot="1">
       <c r="B176" s="35" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C176" s="36" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D176" s="36" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E176" s="36" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F176" s="36" t="n">
         <v>9600</v>
@@ -7208,7 +7224,7 @@
       <c r="J176" s="54" t="n"/>
       <c r="K176" s="147" t="n"/>
       <c r="L176" s="173" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="M176" s="147" t="n"/>
     </row>
@@ -7232,16 +7248,16 @@
     </row>
     <row r="179" spans="1:22">
       <c r="B179" s="91" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C179" s="91" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D179" s="91" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E179" s="91" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F179" s="91" t="n">
         <v>30000</v>
@@ -7251,55 +7267,55 @@
       <c r="I179" s="128" t="n"/>
       <c r="J179" s="128" t="n"/>
       <c r="L179" s="173" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:22">
       <c r="B180" s="91" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C180" s="91" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D180" s="91" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E180" s="91" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F180" s="91" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G180" s="91" t="n"/>
       <c r="H180" s="128" t="n"/>
       <c r="I180" s="128" t="n"/>
       <c r="J180" s="128" t="n"/>
       <c r="L180" s="173" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="181" spans="1:22">
       <c r="B181" s="91" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C181" s="91" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D181" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="E181" s="91" t="s">
+        <v>248</v>
+      </c>
+      <c r="F181" s="91" t="s">
         <v>249</v>
-      </c>
-      <c r="E181" s="91" t="s">
-        <v>246</v>
-      </c>
-      <c r="F181" s="91" t="s">
-        <v>247</v>
       </c>
       <c r="G181" s="91" t="n"/>
       <c r="H181" s="128" t="n"/>
       <c r="I181" s="128" t="n"/>
       <c r="J181" s="128" t="n"/>
       <c r="L181" s="173" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="182" spans="1:22">
@@ -7316,40 +7332,40 @@
     </row>
     <row r="183" spans="1:22">
       <c r="B183" s="91" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C183" s="91" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D183" s="91" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E183" s="91" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F183" s="91" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G183" s="91" t="n"/>
       <c r="H183" s="128" t="n"/>
       <c r="I183" s="128" t="n"/>
       <c r="J183" s="128" t="n"/>
       <c r="L183" s="173" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="184" spans="1:22">
       <c r="B184" s="91" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C184" s="91" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D184" s="91" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E184" s="91" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F184" s="91" t="n">
         <v>3000</v>
@@ -7359,7 +7375,7 @@
       <c r="I184" s="128" t="n"/>
       <c r="J184" s="128" t="n"/>
       <c r="L184" s="173" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="185" spans="1:22">
@@ -7376,50 +7392,50 @@
     </row>
     <row r="186" spans="1:22">
       <c r="B186" s="91" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C186" s="91" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D186" s="91" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E186" s="91" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F186" s="91" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G186" s="91" t="n"/>
       <c r="H186" s="128" t="n"/>
       <c r="I186" s="128" t="n"/>
       <c r="J186" s="128" t="n"/>
       <c r="L186" s="173" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="187" spans="1:22">
       <c r="B187" s="91" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C187" s="91" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D187" s="91" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E187" s="91" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F187" s="91" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G187" s="91" t="n"/>
       <c r="H187" s="128" t="n"/>
       <c r="I187" s="128" t="n"/>
       <c r="J187" s="128" t="n"/>
       <c r="L187" s="173" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row customHeight="1" ht="13.5" r="188" s="140" spans="1:22" thickBot="1">
@@ -7434,7 +7450,7 @@
       <c r="B189" s="28" t="n"/>
       <c r="C189" s="29" t="n"/>
       <c r="D189" s="149" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F189" s="29" t="n"/>
       <c r="G189" s="29" t="n"/>
@@ -7445,16 +7461,16 @@
     </row>
     <row customHeight="1" ht="13.5" r="190" s="140" spans="1:22" thickBot="1">
       <c r="B190" s="130" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C190" s="131" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D190" s="131" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E190" s="131" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F190" s="131" t="n">
         <v>500</v>
@@ -7464,7 +7480,7 @@
       <c r="I190" s="53" t="n"/>
       <c r="J190" s="54" t="n"/>
       <c r="L190" s="173" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" spans="1:22">
@@ -7551,14 +7567,14 @@
     <row r="198" spans="1:22">
       <c r="A198" s="120" t="n"/>
       <c r="B198" s="165" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G198" s="114" t="n"/>
       <c r="H198" s="128" t="n"/>
       <c r="I198" s="128" t="n"/>
       <c r="J198" s="128" t="n"/>
       <c r="L198" s="173" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row customHeight="1" ht="13.5" r="199" s="140" spans="1:22">
@@ -7597,7 +7613,7 @@
       <c r="B202" s="33" t="n"/>
       <c r="C202" s="149" t="n"/>
       <c r="D202" s="163" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F202" s="149" t="n"/>
       <c r="G202" s="149" t="n"/>
@@ -7608,7 +7624,7 @@
     </row>
     <row r="203" spans="1:22">
       <c r="B203" s="162" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G203" s="153" t="n"/>
       <c r="H203" s="128" t="n"/>
@@ -7630,50 +7646,50 @@
     </row>
     <row r="205" spans="1:22">
       <c r="B205" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C205" s="91" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D205" s="91" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E205" s="72" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F205" s="72" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G205" s="72" t="n"/>
       <c r="H205" s="128" t="n"/>
       <c r="I205" s="128" t="n"/>
       <c r="J205" s="51" t="n"/>
       <c r="L205" s="173" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="206" spans="1:22">
       <c r="B206" s="30" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C206" s="91" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D206" s="91" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E206" s="91" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F206" s="91" t="s">
-        <v>283</v>
+        <v>64</v>
       </c>
       <c r="G206" s="91" t="n"/>
       <c r="H206" s="128" t="n"/>
       <c r="I206" s="128" t="n"/>
       <c r="J206" s="51" t="n"/>
       <c r="L206" s="173" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="207" spans="1:22">
@@ -7681,7 +7697,7 @@
       <c r="C207" s="91" t="n"/>
       <c r="D207" s="91" t="n"/>
       <c r="E207" s="91" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F207" s="91" t="n">
         <v>0</v>
@@ -7691,7 +7707,7 @@
       <c r="I207" s="128" t="n"/>
       <c r="J207" s="51" t="n"/>
       <c r="L207" s="173" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="208" spans="1:22">
@@ -7699,7 +7715,7 @@
       <c r="C208" s="91" t="n"/>
       <c r="D208" s="91" t="n"/>
       <c r="E208" s="91" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F208" s="91" t="n">
         <v>35</v>
@@ -7709,7 +7725,7 @@
       <c r="I208" s="128" t="n"/>
       <c r="J208" s="51" t="n"/>
       <c r="L208" s="173" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="209" spans="1:22">
@@ -7717,7 +7733,7 @@
       <c r="C209" s="91" t="n"/>
       <c r="D209" s="91" t="n"/>
       <c r="E209" s="91" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F209" s="91" t="n">
         <v>15</v>
@@ -7727,7 +7743,7 @@
       <c r="I209" s="128" t="n"/>
       <c r="J209" s="51" t="n"/>
       <c r="L209" s="173" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="210" spans="1:22">
@@ -7735,7 +7751,7 @@
       <c r="C210" s="91" t="n"/>
       <c r="D210" s="91" t="n"/>
       <c r="E210" s="91" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F210" s="91" t="n">
         <v>249</v>
@@ -7745,7 +7761,7 @@
       <c r="I210" s="128" t="n"/>
       <c r="J210" s="51" t="n"/>
       <c r="L210" s="173" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="211" spans="1:22">
@@ -7753,7 +7769,7 @@
       <c r="C211" s="91" t="n"/>
       <c r="D211" s="91" t="n"/>
       <c r="E211" s="91" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F211" s="91" t="n">
         <v>3</v>
@@ -7763,7 +7779,7 @@
       <c r="I211" s="128" t="n"/>
       <c r="J211" s="51" t="n"/>
       <c r="L211" s="173" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
     </row>
     <row r="212" spans="1:22">
@@ -7771,7 +7787,7 @@
       <c r="C212" s="91" t="n"/>
       <c r="D212" s="91" t="n"/>
       <c r="E212" s="91" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F212" s="91" t="n">
         <v>10</v>
@@ -7781,7 +7797,7 @@
       <c r="I212" s="128" t="n"/>
       <c r="J212" s="51" t="n"/>
       <c r="L212" s="173" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
     </row>
     <row r="213" spans="1:22">
@@ -7789,7 +7805,7 @@
       <c r="C213" s="91" t="n"/>
       <c r="D213" s="91" t="n"/>
       <c r="E213" s="91" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F213" s="91" t="n">
         <v>10</v>
@@ -7799,7 +7815,7 @@
       <c r="I213" s="128" t="n"/>
       <c r="J213" s="51" t="n"/>
       <c r="L213" s="173" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
     </row>
     <row r="214" spans="1:22">
@@ -7807,7 +7823,7 @@
       <c r="C214" s="91" t="n"/>
       <c r="D214" s="91" t="n"/>
       <c r="E214" s="91" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F214" s="91" t="n">
         <v>400</v>
@@ -7817,7 +7833,7 @@
       <c r="I214" s="128" t="n"/>
       <c r="J214" s="51" t="n"/>
       <c r="L214" s="173" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="215" spans="1:22">
@@ -7825,7 +7841,7 @@
       <c r="C215" s="91" t="n"/>
       <c r="D215" s="91" t="n"/>
       <c r="E215" s="91" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F215" s="91" t="n">
         <v>400</v>
@@ -7835,7 +7851,7 @@
       <c r="I215" s="128" t="n"/>
       <c r="J215" s="51" t="n"/>
       <c r="L215" s="173" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row customHeight="1" ht="13.5" r="216" s="140" spans="1:22" thickBot="1">
@@ -7843,22 +7859,24 @@
         <v>29</v>
       </c>
       <c r="C216" s="32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D216" s="32" t="s">
         <v>31</v>
       </c>
       <c r="E216" s="32" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F216" s="32" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G216" s="32" t="n"/>
       <c r="H216" s="52" t="n"/>
       <c r="I216" s="53" t="n"/>
       <c r="J216" s="54" t="n"/>
-      <c r="L216" s="173" t="n"/>
+      <c r="L216" s="173" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="217" spans="1:22">
       <c r="B217" s="91" t="n"/>
@@ -7887,14 +7905,14 @@
     <row r="219" spans="1:22">
       <c r="A219" s="120" t="n"/>
       <c r="B219" s="151" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G219" s="123" t="n"/>
       <c r="H219" s="128" t="n"/>
       <c r="I219" s="128" t="n"/>
       <c r="J219" s="128" t="n"/>
       <c r="L219" s="173" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row customHeight="1" ht="13.5" r="220" s="140" spans="1:22">
@@ -7916,14 +7934,14 @@
     <row r="222" spans="1:22">
       <c r="A222" s="120" t="n"/>
       <c r="B222" s="151" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G222" s="123" t="n"/>
       <c r="H222" s="128" t="n"/>
       <c r="I222" s="128" t="n"/>
       <c r="J222" s="128" t="n"/>
       <c r="L222" s="173" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row customHeight="1" ht="13.5" r="223" s="140" spans="1:22">
@@ -8722,18 +8740,18 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="E2" s="38" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="D4" s="37" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8744,13 +8762,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8758,13 +8776,13 @@
         <v>2</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8772,13 +8790,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -8786,13 +8804,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -8800,13 +8818,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -8814,10 +8832,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8825,10 +8843,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -8836,10 +8854,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -8847,10 +8865,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -8858,10 +8876,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -8869,10 +8887,10 @@
         <v>11</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -8880,10 +8898,10 @@
         <v>12</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8891,10 +8909,10 @@
         <v>13</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -8902,10 +8920,10 @@
         <v>14</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -8913,10 +8931,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -8924,10 +8942,10 @@
         <v>16</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -8935,7 +8953,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -8943,7 +8961,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -8951,7 +8969,7 @@
         <v>19</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:6">

</xml_diff>